<commit_message>
Un-nesting test models setup and data files to allow testing them. Revising models for testing. Still work to do.
</commit_message>
<xml_diff>
--- a/tests/integration/models/2b - planning_discounting/concept.xlsx
+++ b/tests/integration/models/2b - planning_discounting/concept.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\2b - planning_discounting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\models\2b - planning_discounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C40F4BA-9AD0-4ED8-B14F-16CC6A9550D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358A3296-B010-47F0-A517-EC0E83F8CF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="concept" sheetId="3" r:id="rId1"/>
@@ -20,16 +20,16 @@
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">concept!$F$21:$F$25,concept!$J$21:$K$25,concept!$H$21:$H$25</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">concept!$F$21:$F$25,concept!$H$21:$H$25,concept!$J$21:$J$25</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">concept!$V$10:$Z$10</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">concept!$F$21:$F$25</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">concept!$H$21:$H$25</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">concept!$H$21:$H$25</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">concept!$H$29:$H$33</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">concept!$V$8:$Z$8</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">concept!$V$8:$Z$8</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">concept!$H$21:$H$25</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
@@ -38,21 +38,21 @@
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">concept!$P$12</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">concept!$H$37:$H$41</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">concept!$H$21:$H$25</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">concept!$H$37:$H$41</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">concept!$H$29:$H$33</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -374,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -392,9 +392,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -405,10 +402,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -699,37 +694,37 @@
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W11" sqref="W11"/>
+      <selection pane="bottomRight" activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="12" width="7.42578125" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" customWidth="1"/>
-    <col min="15" max="15" width="4.85546875" customWidth="1"/>
-    <col min="16" max="17" width="7.42578125" customWidth="1"/>
-    <col min="18" max="19" width="5.7109375" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" customWidth="1"/>
-    <col min="21" max="26" width="7.42578125" customWidth="1"/>
-    <col min="27" max="45" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" customWidth="1"/>
+    <col min="7" max="7" width="4.7265625" customWidth="1"/>
+    <col min="8" max="8" width="6.81640625" customWidth="1"/>
+    <col min="9" max="9" width="4.7265625" customWidth="1"/>
+    <col min="10" max="12" width="7.453125" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.26953125" customWidth="1"/>
+    <col min="15" max="15" width="4.81640625" customWidth="1"/>
+    <col min="16" max="17" width="7.453125" customWidth="1"/>
+    <col min="18" max="19" width="5.7265625" customWidth="1"/>
+    <col min="20" max="20" width="6.7265625" customWidth="1"/>
+    <col min="21" max="26" width="7.453125" customWidth="1"/>
+    <col min="27" max="45" width="6.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -764,7 +759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -772,7 +767,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -795,7 +790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>10</v>
       </c>
@@ -803,10 +798,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
@@ -817,7 +812,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -842,24 +837,24 @@
       <c r="N8" s="12">
         <v>207</v>
       </c>
-      <c r="V8" s="17" cm="1">
+      <c r="V8" s="16" cm="1">
         <f t="array" ref="V8:Z8">TRANSPOSE(F21:F25)-MMULT(H8:H8,TRANSPOSE(H21:H25))-J8:N8</f>
         <v>-9.9999999747524271E-7</v>
       </c>
-      <c r="W8" s="18">
+      <c r="W8" s="17">
         <v>-3.0000000066365828E-6</v>
       </c>
-      <c r="X8" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="18">
+      <c r="X8" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="17">
         <v>-1.9999999949504854E-6</v>
       </c>
-      <c r="Z8" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z8" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
@@ -870,7 +865,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>9</v>
       </c>
@@ -888,29 +883,29 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="V10" s="21" cm="1">
+      <c r="V10" s="19" cm="1">
         <f t="array" ref="V10:Z10">TRANSPOSE(H21:H25)-MMULT(F10:F10,TRANSPOSE(F21:F25))</f>
         <v>0</v>
       </c>
-      <c r="W10" s="18">
-        <v>0</v>
-      </c>
-      <c r="X10" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W10" s="17">
+        <v>0</v>
+      </c>
+      <c r="X10" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="P11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>17</v>
       </c>
@@ -922,11 +917,11 @@
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="9">
-        <f>SUM(_xlfn.ANCHORARRAY(Q21),_xlfn.ANCHORARRAY(Q29))</f>
-        <v>1198.4127100000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+        <f>SUM(Q21:Q25,Q29:Q33)</f>
+        <v>3315.3077913961265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>19</v>
       </c>
@@ -937,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>21</v>
       </c>
@@ -948,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="G15" s="8" t="s">
         <v>23</v>
       </c>
@@ -956,7 +951,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>24</v>
       </c>
@@ -967,7 +962,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F19" s="3" t="s">
         <v>26</v>
       </c>
@@ -978,16 +973,16 @@
       <c r="J19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
       <c r="Q19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="F20" t="s">
         <v>14</v>
       </c>
@@ -1004,7 +999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1017,10 +1012,7 @@
       <c r="J21" s="10">
         <v>108.73016</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="14" cm="1">
+      <c r="M21" s="13" cm="1">
         <f t="array" ref="M21:M25">MMULT(J21:J25,_xlfn.MUNIT(1)*H12:H12)</f>
         <v>1087.3016</v>
       </c>
@@ -1029,7 +1021,7 @@
         <v>1087.3016</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1041,9 +1033,6 @@
       </c>
       <c r="J22" s="10">
         <v>31.746032</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
       </c>
       <c r="M22" s="6">
         <v>317.46032000000002</v>
@@ -1053,7 +1042,7 @@
         <v>302.34316190476193</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1065,9 +1054,6 @@
       </c>
       <c r="J23" s="10">
         <v>38.095238000000002</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
       </c>
       <c r="M23" s="6">
         <v>380.95238000000001</v>
@@ -1077,7 +1063,7 @@
         <v>345.53503854875282</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1089,9 +1075,6 @@
       </c>
       <c r="J24" s="10">
         <v>46.031745999999998</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
       </c>
       <c r="M24" s="6">
         <v>460.31745999999998</v>
@@ -1101,7 +1084,7 @@
         <v>397.63952920850875</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1113,9 +1096,6 @@
       </c>
       <c r="J25" s="10">
         <v>53.968254000000002</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
       </c>
       <c r="M25" s="6">
         <v>539.68254000000002</v>
@@ -1125,24 +1105,22 @@
         <v>443.99816125996887</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="F26" s="7"/>
       <c r="H26" s="7"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="20" t="s">
+    </row>
+    <row r="27" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G27" s="15"/>
+      <c r="H27" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="13" t="s">
+      <c r="I27" s="15"/>
+      <c r="J27" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
       <c r="M27" s="3" t="s">
         <v>31</v>
       </c>
@@ -1151,30 +1129,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H28" s="15" t="s">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="H28" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="J28" s="14" t="s">
         <v>9</v>
       </c>
       <c r="L28" s="3"/>
-      <c r="M28" s="15" t="s">
+      <c r="M28" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Q28" s="15" t="s">
+      <c r="Q28" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="H29" s="11" cm="1">
-        <f t="array" ref="H29:I33">J29:K33*H14:H14</f>
-        <v>0</v>
-      </c>
-      <c r="I29">
+      <c r="H29" s="11">
+        <f t="array" ref="H29:H33">J29:J33*H14</f>
         <v>0</v>
       </c>
       <c r="J29" s="6" cm="1">
@@ -1190,14 +1165,11 @@
         <v>111.11111</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="H30" s="11">
-        <v>0</v>
-      </c>
-      <c r="I30">
         <v>0</v>
       </c>
       <c r="J30" s="6">
@@ -1211,14 +1183,11 @@
         <v>126.98412380952379</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>3</v>
       </c>
       <c r="H31" s="11">
-        <v>0</v>
-      </c>
-      <c r="I31">
         <v>0</v>
       </c>
       <c r="J31" s="6">
@@ -1232,14 +1201,11 @@
         <v>145.12471655328798</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>4</v>
       </c>
       <c r="H32" s="11">
-        <v>0</v>
-      </c>
-      <c r="I32">
         <v>0</v>
       </c>
       <c r="J32" s="6">
@@ -1253,14 +1219,11 @@
         <v>166.04878090918905</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="H33" s="11">
-        <v>0</v>
-      </c>
-      <c r="I33">
         <v>0</v>
       </c>
       <c r="J33" s="6">
@@ -1274,17 +1237,17 @@
         <v>189.22156920213286</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H35" s="13" t="s">
+    <row r="35" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H35" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I35" s="13"/>
+      <c r="I35" s="20"/>
       <c r="O35" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H36" s="15" t="s">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="H36" s="14" t="s">
         <v>9</v>
       </c>
       <c r="O36" t="s">
@@ -1303,17 +1266,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
-      <c r="H37" s="6" cm="1">
-        <f t="array" ref="H37:I41">J29:K33*H15:H15</f>
+      <c r="H37" s="6">
+        <f t="array" ref="H37:H41">J29:J33*H15</f>
         <v>111.11111200000001</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
       <c r="O37" s="4">
         <v>1</v>
       </c>
@@ -1330,16 +1290,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2</v>
       </c>
       <c r="H38" s="6">
         <v>133.33333439999998</v>
       </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
       <c r="O38" s="4">
         <v>1</v>
       </c>
@@ -1356,16 +1313,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>3</v>
       </c>
       <c r="H39" s="6">
         <v>160.000001</v>
       </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
       <c r="O39" s="4">
         <v>1</v>
       </c>
@@ -1382,16 +1336,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>4</v>
       </c>
       <c r="H40" s="6">
         <v>192.22222319999997</v>
       </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
       <c r="O40" s="4">
         <v>1</v>
       </c>
@@ -1408,16 +1359,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
       <c r="H41" s="6">
         <v>230.00000099999997</v>
       </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
       <c r="O41" s="4">
         <v>1</v>
       </c>
@@ -1434,18 +1382,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L43" s="16"/>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
+    <row r="43" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="M19:O19"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Contents!A1" display="Back to contents" xr:uid="{368E31E9-B2F2-477E-87DF-24E3969516DC}"/>
   </hyperlinks>

</xml_diff>